<commit_message>
cleaned up fofm allocation script and added krill to fish meal
</commit_message>
<xml_diff>
--- a/data/tidy_data/allocation/embodied_fish_allocation.xlsx
+++ b/data/tidy_data/allocation/embodied_fish_allocation.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26502"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gclawson/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B568B7E-0DF5-CD43-9A2D-F3AD4056BB27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{418A9C87-76E1-43D3-AFF3-D6E1E7390878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37380" yWindow="1780" windowWidth="33580" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,10 +17,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="66">
   <si>
     <t>species</t>
   </si>
@@ -62,6 +57,12 @@
     <t>mass_value</t>
   </si>
   <si>
+    <t>CommonName</t>
+  </si>
+  <si>
+    <t>sci_name</t>
+  </si>
+  <si>
     <t>Gross energy MJ kg-1 DM</t>
   </si>
   <si>
@@ -83,12 +84,24 @@
     <t>SO</t>
   </si>
   <si>
+    <t>Antarctic krill</t>
+  </si>
+  <si>
+    <t>Euphausia superba</t>
+  </si>
+  <si>
     <t>Atlantic herring (Clupea harengus) b</t>
   </si>
   <si>
     <t>IS</t>
   </si>
   <si>
+    <t>Atlantic herring</t>
+  </si>
+  <si>
+    <t>Clupea harengus</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atlantic herring (C. harengus) b </t>
   </si>
   <si>
@@ -101,18 +114,42 @@
     <t>Atlantic mackerel (Scomber scombrus) b</t>
   </si>
   <si>
+    <t>Atlantic mackerel</t>
+  </si>
+  <si>
+    <t>Scomber scombrus</t>
+  </si>
+  <si>
     <t>Blue whiting (Micromesistius poutassou) b</t>
   </si>
   <si>
+    <t>Blue whiting</t>
+  </si>
+  <si>
+    <t>Micromesistius poutassou</t>
+  </si>
+  <si>
     <t>Boarfish (Capros aper) b</t>
   </si>
   <si>
+    <t>Boarfish</t>
+  </si>
+  <si>
+    <t>Capros aper</t>
+  </si>
+  <si>
     <t>Capelin (Mallotus villosus) b</t>
   </si>
   <si>
     <t>BS</t>
   </si>
   <si>
+    <t>Capelin</t>
+  </si>
+  <si>
+    <t>Mallotus villosus</t>
+  </si>
+  <si>
     <t>Capelin (M. villosus) b</t>
   </si>
   <si>
@@ -122,25 +159,67 @@
     <t>HC</t>
   </si>
   <si>
+    <t>Chilean jack</t>
+  </si>
+  <si>
+    <t>Trachurus murphyi</t>
+  </si>
+  <si>
     <t>European sprat (Sprattus sprattus) b</t>
   </si>
   <si>
+    <t>European sprat</t>
+  </si>
+  <si>
+    <t>Sprattus sprattus</t>
+  </si>
+  <si>
     <t>Gulf menhaden (Brevoorti patronus) b</t>
   </si>
   <si>
     <t>GM</t>
   </si>
   <si>
+    <t>Gulf menhaden</t>
+  </si>
+  <si>
+    <t>Brevoortia patronus</t>
+  </si>
+  <si>
     <t>Norway pout (Trisopterus esmarkii) b</t>
   </si>
   <si>
+    <t>Norway pout</t>
+  </si>
+  <si>
+    <t>Trisopterus esmarkii</t>
+  </si>
+  <si>
     <t>Peruvian bnchovy (Engraulis ringens) b</t>
   </si>
   <si>
+    <t>Peruvian anchovy</t>
+  </si>
+  <si>
+    <t>Engraulis ringens</t>
+  </si>
+  <si>
     <t>Sandeels (Ammodytes tobianus) b</t>
   </si>
   <si>
+    <t>Sandeels</t>
+  </si>
+  <si>
+    <t>Ammodytes tobianus</t>
+  </si>
+  <si>
     <t>South American pilchard (Sardinops sagax) b</t>
+  </si>
+  <si>
+    <t>South American pilchard</t>
+  </si>
+  <si>
+    <t>Sardinops sagax</t>
   </si>
   <si>
     <t>Global average c</t>
@@ -156,7 +235,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +247,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F2328"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -211,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,6 +314,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,20 +635,22 @@
   <dimension ref="A1:AI74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="4" width="9.1640625" style="7"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="7"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -587,8 +678,12 @@
       <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -614,21 +709,21 @@
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
@@ -636,8 +731,12 @@
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="J2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -663,21 +762,21 @@
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
@@ -685,8 +784,12 @@
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -712,12 +815,12 @@
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6">
         <v>0.16</v>
@@ -726,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2">
         <f>(C4*$G$2)/SUM((C4*$G$2),($G$3*D4))</f>
@@ -744,8 +847,12 @@
         <f>H4/C4</f>
         <v>6.25</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="J4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -771,12 +878,12 @@
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6">
         <v>0.16</v>
@@ -785,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2">
         <f>(D5*$G$3)/SUM((D5*$G$3),(C5*$G$2))</f>
@@ -801,8 +908,12 @@
       <c r="I5" s="6">
         <v>0</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="J5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -828,12 +939,12 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="15.75">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6">
         <v>0.2</v>
@@ -842,7 +953,7 @@
         <v>0.12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F6" s="2">
         <f>(C6*$G$2)/SUM((C6*$G$2),($G$3*D6))</f>
@@ -860,8 +971,12 @@
         <f>H6/C6</f>
         <v>3.125</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -887,12 +1002,12 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <v>0.2</v>
@@ -901,7 +1016,7 @@
         <v>0.12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2">
         <f>(D7*$G$3)/SUM((D7*$G$3),(C7*$G$2))</f>
@@ -919,8 +1034,12 @@
         <f>H7/D7</f>
         <v>3.125</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="J7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -946,12 +1065,12 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C8" s="6">
         <v>0.2</v>
@@ -960,7 +1079,7 @@
         <v>0.12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2">
         <f>(C8*$G$2)/SUM((C8*$G$2),($G$3*D8))</f>
@@ -978,8 +1097,12 @@
         <f>H8/C8</f>
         <v>3.125</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="J8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1005,12 +1128,12 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C9" s="6">
         <v>0.2</v>
@@ -1019,7 +1142,7 @@
         <v>0.12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F9" s="2">
         <f>(D9*$G$3)/SUM((D9*$G$3),(C9*$G$2))</f>
@@ -1037,8 +1160,12 @@
         <f>H9/D9</f>
         <v>3.125</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1064,12 +1191,12 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C10" s="6">
         <v>0.2</v>
@@ -1078,7 +1205,7 @@
         <v>0.12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2">
         <f>(C10*$G$2)/SUM((C10*$G$2),($G$3*D10))</f>
@@ -1096,8 +1223,12 @@
         <f>H10/C10</f>
         <v>3.125</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="J10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1123,12 +1254,12 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6">
         <v>0.2</v>
@@ -1137,7 +1268,7 @@
         <v>0.12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2">
         <f>(D11*$G$3)/SUM((D11*$G$3),(C11*$G$2))</f>
@@ -1155,8 +1286,12 @@
         <f>H11/D11</f>
         <v>3.125</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="J11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1182,12 +1317,12 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="15.75">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C12" s="6">
         <v>0.19</v>
@@ -1196,7 +1331,7 @@
         <v>0.19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2">
         <f>(C12*$G$2)/SUM((C12*$G$2),($G$3*D12))</f>
@@ -1214,8 +1349,12 @@
         <f>H12/C12</f>
         <v>2.6315789473684212</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="J12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1241,12 +1380,12 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6">
         <v>0.19</v>
@@ -1255,7 +1394,7 @@
         <v>0.19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F13" s="2">
         <f>(D13*$G$3)/SUM((D13*$G$3),(C13*$G$2))</f>
@@ -1273,8 +1412,12 @@
         <f>H13/D13</f>
         <v>2.6315789473684212</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="J13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1300,12 +1443,12 @@
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="15.75">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C14" s="6">
         <v>0.2</v>
@@ -1314,7 +1457,7 @@
         <v>0.02</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F14" s="2">
         <f>(C14*$G$2)/SUM((C14*$G$2),($G$3*D14))</f>
@@ -1332,8 +1475,12 @@
         <f>H14/C14</f>
         <v>4.5454545454545459</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="J14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1359,12 +1506,12 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6">
         <v>0.2</v>
@@ -1373,7 +1520,7 @@
         <v>0.02</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F15" s="2">
         <f>(D15*$G$3)/SUM((D15*$G$3),(C15*$G$2))</f>
@@ -1391,8 +1538,12 @@
         <f>H15/D15</f>
         <v>4.5454545454545459</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="J15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>32</v>
+      </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1418,12 +1569,12 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="15.75">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C16" s="6">
         <v>0.22</v>
@@ -1432,7 +1583,7 @@
         <v>0.03</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F16" s="2">
         <f>(C16*$G$2)/SUM((C16*$G$2),($G$3*D16))</f>
@@ -1450,8 +1601,12 @@
         <f>H16/C16</f>
         <v>4</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="J16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>35</v>
+      </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1477,12 +1632,12 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" ht="15.75">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C17" s="6">
         <v>0.22</v>
@@ -1491,7 +1646,7 @@
         <v>0.03</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F17" s="2">
         <f>(D17*$G$3)/SUM((D17*$G$3),(C17*$G$2))</f>
@@ -1509,8 +1664,12 @@
         <f>H17/D17</f>
         <v>4</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="J17" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>35</v>
+      </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1536,12 +1695,12 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" ht="15.75">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C18" s="6">
         <v>0.17</v>
@@ -1550,7 +1709,7 @@
         <v>0.08</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F18" s="2">
         <f>(C18*$G$2)/SUM((C18*$G$2),($G$3*D18))</f>
@@ -1568,8 +1727,12 @@
         <f>H18/C18</f>
         <v>4</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="J18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1595,12 +1758,12 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C19" s="6">
         <v>0.17</v>
@@ -1609,7 +1772,7 @@
         <v>0.08</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F19" s="2">
         <f>(D19*$G$3)/SUM((D19*$G$3),(C19*$G$2))</f>
@@ -1627,8 +1790,12 @@
         <f>H19/D19</f>
         <v>4</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="J19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1654,12 +1821,12 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C20" s="6">
         <v>0.17</v>
@@ -1668,7 +1835,7 @@
         <v>0.08</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F20" s="2">
         <f>(C20*$G$2)/SUM((C20*$G$2),($G$3*D20))</f>
@@ -1686,8 +1853,12 @@
         <f>H20/C20</f>
         <v>4</v>
       </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="J20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1713,12 +1884,12 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" ht="15.75">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C21" s="6">
         <v>0.17</v>
@@ -1727,7 +1898,7 @@
         <v>0.08</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F21" s="2">
         <f>(D21*$G$3)/SUM((D21*$G$3),(C21*$G$2))</f>
@@ -1745,8 +1916,12 @@
         <f>H21/D21</f>
         <v>4</v>
       </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="J21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1772,12 +1947,12 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" ht="15.75">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C22" s="6">
         <v>0.19</v>
@@ -1786,7 +1961,7 @@
         <v>0.19</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F22" s="2">
         <f>(C22*$G$2)/SUM((C22*$G$2),($G$3*D22))</f>
@@ -1804,8 +1979,12 @@
         <f>H22/C22</f>
         <v>2.6315789473684212</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="J22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1831,12 +2010,12 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" ht="15.75">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C23" s="6">
         <v>0.19</v>
@@ -1845,7 +2024,7 @@
         <v>0.19</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F23" s="2">
         <f>(D23*$G$3)/SUM((D23*$G$3),(C23*$G$2))</f>
@@ -1863,8 +2042,12 @@
         <f>H23/D23</f>
         <v>2.6315789473684212</v>
       </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="J23" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1890,12 +2073,12 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" ht="15.75">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C24" s="6">
         <v>0.19</v>
@@ -1904,7 +2087,7 @@
         <v>0.08</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F24" s="2">
         <f>(C24*$G$2)/SUM((C24*$G$2),($G$3*D24))</f>
@@ -1922,8 +2105,12 @@
         <f>H24/C24</f>
         <v>3.7037037037037037</v>
       </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="J24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -1949,12 +2136,12 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" ht="15.75">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C25" s="6">
         <v>0.19</v>
@@ -1963,7 +2150,7 @@
         <v>0.08</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F25" s="2">
         <f>(D25*$G$3)/SUM((D25*$G$3),(C25*$G$2))</f>
@@ -1981,8 +2168,12 @@
         <f>H25/D25</f>
         <v>3.7037037037037033</v>
       </c>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="J25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2008,12 +2199,12 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" ht="15.75">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C26" s="6">
         <v>0.24</v>
@@ -2022,7 +2213,7 @@
         <v>0.13</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F26" s="2">
         <f>(C26*$G$2)/SUM((C26*$G$2),($G$3*D26))</f>
@@ -2040,8 +2231,12 @@
         <f>H26/C26</f>
         <v>2.7027027027027031</v>
       </c>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="J26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -2067,12 +2262,12 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" ht="15.75">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C27" s="6">
         <v>0.24</v>
@@ -2081,7 +2276,7 @@
         <v>0.13</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F27" s="2">
         <f>(D27*$G$3)/SUM((D27*$G$3),(C27*$G$2))</f>
@@ -2099,8 +2294,12 @@
         <f>H27/D27</f>
         <v>2.7027027027027026</v>
       </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="J27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2126,12 +2325,12 @@
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" ht="15.75">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C28" s="6">
         <v>0.2</v>
@@ -2140,7 +2339,7 @@
         <v>0.12</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F28" s="2">
         <f>(C28*$G$2)/SUM((C28*$G$2),($G$3*D28))</f>
@@ -2158,8 +2357,12 @@
         <f>H28/C28</f>
         <v>3.125</v>
       </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="J28" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -2185,12 +2388,12 @@
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" ht="15.75">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C29" s="6">
         <v>0.2</v>
@@ -2199,7 +2402,7 @@
         <v>0.12</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F29" s="2">
         <f>(D29*$G$3)/SUM((D29*$G$3),(C29*$G$2))</f>
@@ -2217,8 +2420,12 @@
         <f>H29/D29</f>
         <v>3.125</v>
       </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="J29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2244,12 +2451,12 @@
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" ht="15.75">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C30" s="6">
         <v>0.23</v>
@@ -2258,7 +2465,7 @@
         <v>0.05</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F30" s="2">
         <f>(C30*$G$2)/SUM((C30*$G$2),($G$3*D30))</f>
@@ -2276,8 +2483,12 @@
         <f>H30/C30</f>
         <v>3.5714285714285712</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="J30" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>57</v>
+      </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -2303,12 +2514,12 @@
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" ht="15.75">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C31" s="6">
         <v>0.23</v>
@@ -2317,7 +2528,7 @@
         <v>0.05</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F31" s="2">
         <f>(D31*$G$3)/SUM((D31*$G$3),(C31*$G$2))</f>
@@ -2335,8 +2546,12 @@
         <f>H31/D31</f>
         <v>3.5714285714285712</v>
       </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="J31" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>57</v>
+      </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2362,12 +2577,12 @@
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" ht="15.75">
       <c r="A32" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C32" s="6">
         <v>0.2</v>
@@ -2376,7 +2591,7 @@
         <v>0.04</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F32" s="2">
         <f>(C32*$G$2)/SUM((C32*$G$2),($G$3*D32))</f>
@@ -2394,8 +2609,12 @@
         <f>H32/C32</f>
         <v>4.1666666666666661</v>
       </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="J32" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2421,12 +2640,12 @@
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35" ht="15.75">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C33" s="6">
         <v>0.2</v>
@@ -2435,7 +2654,7 @@
         <v>0.04</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F33" s="2">
         <f>(D33*$G$3)/SUM((D33*$G$3),(C33*$G$2))</f>
@@ -2453,8 +2672,12 @@
         <f>H33/D33</f>
         <v>4.1666666666666661</v>
       </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="J33" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2480,12 +2703,12 @@
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35" ht="15.75">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C34" s="6">
         <v>0.23</v>
@@ -2494,7 +2717,7 @@
         <v>0.18</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F34" s="2">
         <f>(C34*$G$2)/SUM((C34*$G$2),($G$3*D34))</f>
@@ -2512,8 +2735,12 @@
         <f>H34/C34</f>
         <v>2.4390243902439019</v>
       </c>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="J34" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2539,12 +2766,12 @@
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35" ht="15.75">
       <c r="A35" s="2" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C35" s="6">
         <v>0.23</v>
@@ -2553,7 +2780,7 @@
         <v>0.18</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F35" s="2">
         <f>(D35*$G$3)/SUM((D35*$G$3),(C35*$G$2))</f>
@@ -2571,8 +2798,12 @@
         <f>H35/D35</f>
         <v>2.4390243902439024</v>
       </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="J35" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2598,12 +2829,12 @@
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C36" s="6">
         <v>0.23</v>
@@ -2612,7 +2843,7 @@
         <v>0.05</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F36" s="2">
         <f>(C36*$G$2)/SUM((C36*$G$2),($G$3*D36))</f>
@@ -2630,8 +2861,12 @@
         <f>H36/C36</f>
         <v>3.5714285714285712</v>
       </c>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="J36" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2657,12 +2892,12 @@
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:35">
       <c r="A37" s="3" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C37" s="8">
         <v>0.22500000000000001</v>
@@ -2671,7 +2906,7 @@
         <v>0.05</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F37" s="2">
         <f>(D37*$G$3)/SUM((D37*$G$3),(C37*$G$2))</f>
@@ -2689,8 +2924,12 @@
         <f>H37/D37</f>
         <v>3.6363636363636362</v>
       </c>
-      <c r="J37" s="3"/>
-      <c r="K37" s="4"/>
+      <c r="J37" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="4"/>
@@ -2716,13 +2955,13 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="4"/>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35">
       <c r="B40" s="7"/>
       <c r="D40"/>
       <c r="G40" s="7"/>
       <c r="I40"/>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:35">
       <c r="A41" s="2"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -2733,7 +2972,7 @@
       <c r="H41" s="11"/>
       <c r="I41"/>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:35">
       <c r="A42" s="2"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2744,7 +2983,7 @@
       <c r="H42" s="11"/>
       <c r="I42"/>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:35">
       <c r="A43" s="2"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2755,7 +2994,7 @@
       <c r="H43" s="11"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:35">
       <c r="A44" s="2"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -2766,7 +3005,7 @@
       <c r="H44" s="11"/>
       <c r="I44"/>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:35">
       <c r="A45" s="2"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -2777,7 +3016,7 @@
       <c r="H45" s="11"/>
       <c r="I45"/>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:35">
       <c r="A46" s="2"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -2788,7 +3027,7 @@
       <c r="H46" s="11"/>
       <c r="I46"/>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:35">
       <c r="A47" s="2"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -2799,7 +3038,7 @@
       <c r="H47" s="11"/>
       <c r="I47"/>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:35">
       <c r="A48" s="2"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -2810,7 +3049,7 @@
       <c r="H48" s="11"/>
       <c r="I48"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="2"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -2821,7 +3060,7 @@
       <c r="H49" s="11"/>
       <c r="I49"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="2"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -2832,7 +3071,7 @@
       <c r="H50" s="11"/>
       <c r="I50"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="2"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -2843,7 +3082,7 @@
       <c r="H51" s="11"/>
       <c r="I51"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="2"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -2854,7 +3093,7 @@
       <c r="H52" s="11"/>
       <c r="I52"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="2"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -2865,7 +3104,7 @@
       <c r="H53" s="11"/>
       <c r="I53"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="2"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -2876,7 +3115,7 @@
       <c r="H54" s="11"/>
       <c r="I54"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="2"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -2887,7 +3126,7 @@
       <c r="H55" s="11"/>
       <c r="I55"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="2"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -2898,7 +3137,7 @@
       <c r="H56" s="11"/>
       <c r="I56"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="2"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -2909,7 +3148,7 @@
       <c r="H57" s="11"/>
       <c r="I57"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="2"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -2920,7 +3159,7 @@
       <c r="H58" s="11"/>
       <c r="I58"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9">
       <c r="A59" s="2"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -2931,7 +3170,7 @@
       <c r="H59" s="11"/>
       <c r="I59"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9">
       <c r="A60" s="2"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -2942,7 +3181,7 @@
       <c r="H60" s="11"/>
       <c r="I60"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9">
       <c r="A61" s="2"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -2953,7 +3192,7 @@
       <c r="H61" s="11"/>
       <c r="I61"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9">
       <c r="A62" s="2"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -2964,7 +3203,7 @@
       <c r="H62" s="11"/>
       <c r="I62"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9">
       <c r="A63" s="2"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -2975,7 +3214,7 @@
       <c r="H63" s="11"/>
       <c r="I63"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9">
       <c r="A64" s="2"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -2986,7 +3225,7 @@
       <c r="H64" s="11"/>
       <c r="I64"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9">
       <c r="A65" s="2"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -2997,7 +3236,7 @@
       <c r="H65" s="11"/>
       <c r="I65"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9">
       <c r="A66" s="2"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -3008,7 +3247,7 @@
       <c r="H66" s="11"/>
       <c r="I66"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9">
       <c r="A67" s="2"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -3019,7 +3258,7 @@
       <c r="H67" s="11"/>
       <c r="I67"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9">
       <c r="A68" s="2"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -3030,7 +3269,7 @@
       <c r="H68" s="11"/>
       <c r="I68"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9">
       <c r="A69" s="2"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -3041,7 +3280,7 @@
       <c r="H69" s="11"/>
       <c r="I69"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9">
       <c r="A70" s="2"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -3052,7 +3291,7 @@
       <c r="H70" s="11"/>
       <c r="I70"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9">
       <c r="A71" s="2"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -3063,7 +3302,7 @@
       <c r="H71" s="11"/>
       <c r="I71"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9">
       <c r="A72" s="2"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -3074,7 +3313,7 @@
       <c r="H72" s="11"/>
       <c r="I72"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9">
       <c r="A73" s="2"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -3085,7 +3324,7 @@
       <c r="H73" s="11"/>
       <c r="I73"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9">
       <c r="A74" s="3"/>
       <c r="B74" s="8"/>
       <c r="C74" s="9"/>
@@ -3282,37 +3521,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EE6CB6-2C00-4A2E-B24B-E862454D1C75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EE6CB6-2C00-4A2E-B24B-E862454D1C75}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5A82EE-7F2B-442E-9916-B65751AC8941}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5A82EE-7F2B-442E-9916-B65751AC8941}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A168EB7-056C-45D6-8681-2B21F655F8D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dae89b64-c529-494f-868e-ad5d2094d0fa"/>
-    <ds:schemaRef ds:uri="ed16b9de-937e-42cc-89df-e5a7efc4dd3c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A168EB7-056C-45D6-8681-2B21F655F8D4}"/>
 </file>
</xml_diff>